<commit_message>
Clean up the timing plots
</commit_message>
<xml_diff>
--- a/timing.xlsx
+++ b/timing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johager/Big/Devmountain/assessments/assessment-cs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C65058F1-E3E4-6D42-9174-D9C4BB3FE6B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9694A23E-9381-9845-8925-562AC8D4DB3B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="760" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{65769B2E-A982-8F4E-819A-FAAE07BCE55A}"/>
   </bookViews>
@@ -543,9 +543,7 @@
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -1740,9 +1738,7 @@
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -7647,7 +7643,7 @@
   <dimension ref="B1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7929,7 +7925,7 @@
   <dimension ref="B1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8135,7 +8131,7 @@
   <dimension ref="B1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>